<commit_message>
up n parties: compute ss
</commit_message>
<xml_diff>
--- a/stash size.xlsx
+++ b/stash size.xlsx
@@ -9,12 +9,13 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12210" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12210" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="2 hashes" sheetId="2" r:id="rId1"/>
     <sheet name="3 hashes" sheetId="1" r:id="rId2"/>
-    <sheet name="Sheet1" sheetId="3" r:id="rId3"/>
+    <sheet name="16" sheetId="3" r:id="rId3"/>
+    <sheet name="12" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="171027"/>
   <extLst>
@@ -201,6 +202,104 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>257175</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>437670</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>190300</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Picture 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D32E7FC1-629A-4DD3-AB26-BA7D878FF98E}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="257175" y="114300"/>
+          <a:ext cx="3838095" cy="1600000"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>399619</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>56952</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="Picture 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B737EDD2-F554-4321-BEB5-E173A0900C90}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="3447619" cy="1580952"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1212,8 +1311,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O33"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="O30" sqref="O30"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B31" sqref="B31:F31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1234,23 +1333,23 @@
         <v>0</v>
       </c>
       <c r="B2" s="2">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="C2" s="2">
-        <f>B2+1</f>
-        <v>11</v>
+        <f>B2+4</f>
+        <v>12</v>
       </c>
       <c r="D2" s="2">
-        <f t="shared" ref="D2:F2" si="0">C2+1</f>
-        <v>12</v>
+        <f t="shared" ref="D2:F2" si="0">C2+4</f>
+        <v>16</v>
       </c>
       <c r="E2" s="2">
         <f t="shared" si="0"/>
-        <v>13</v>
+        <v>20</v>
       </c>
       <c r="F2" s="2">
         <f t="shared" si="0"/>
-        <v>14</v>
+        <v>24</v>
       </c>
       <c r="G2" s="1"/>
     </row>
@@ -1258,21 +1357,11 @@
       <c r="A3" s="2">
         <v>20</v>
       </c>
-      <c r="B3" s="3">
-        <v>92</v>
-      </c>
-      <c r="C3" s="3">
-        <v>165</v>
-      </c>
-      <c r="D3" s="3">
-        <v>305</v>
-      </c>
-      <c r="E3" s="3">
-        <v>576</v>
-      </c>
-      <c r="F3" s="3">
-        <v>1113</v>
-      </c>
+      <c r="B3" s="3"/>
+      <c r="C3" s="3"/>
+      <c r="D3" s="3"/>
+      <c r="E3" s="3"/>
+      <c r="F3" s="3"/>
       <c r="G3" s="1"/>
     </row>
     <row r="4" spans="1:13" ht="18.75" x14ac:dyDescent="0.3">
@@ -1344,23 +1433,23 @@
       </c>
       <c r="B9" s="2">
         <f>B2</f>
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="C9" s="2">
         <f t="shared" ref="C9:F9" si="1">C2</f>
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="D9" s="2">
         <f t="shared" si="1"/>
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="E9" s="2">
         <f t="shared" si="1"/>
-        <v>13</v>
+        <v>20</v>
       </c>
       <c r="F9" s="2">
         <f t="shared" si="1"/>
-        <v>14</v>
+        <v>24</v>
       </c>
       <c r="G9" s="1"/>
     </row>
@@ -1369,21 +1458,11 @@
         <f>A3</f>
         <v>20</v>
       </c>
-      <c r="B10" s="3">
-        <v>52</v>
-      </c>
-      <c r="C10" s="3">
-        <v>98</v>
-      </c>
-      <c r="D10" s="3">
-        <v>160</v>
-      </c>
-      <c r="E10" s="3">
-        <v>301</v>
-      </c>
-      <c r="F10" s="3">
-        <v>545</v>
-      </c>
+      <c r="B10" s="3"/>
+      <c r="C10" s="3"/>
+      <c r="D10" s="3"/>
+      <c r="E10" s="3"/>
+      <c r="F10" s="3"/>
       <c r="G10" s="1"/>
     </row>
     <row r="11" spans="1:13" ht="18.75" x14ac:dyDescent="0.3">
@@ -1452,9 +1531,7 @@
       <c r="B17" s="3"/>
       <c r="C17" s="3"/>
       <c r="D17" s="3"/>
-      <c r="E17" s="3">
-        <v>244</v>
-      </c>
+      <c r="E17" s="3"/>
       <c r="F17" s="3"/>
     </row>
     <row r="18" spans="1:15" ht="18.75" x14ac:dyDescent="0.3">
@@ -1496,23 +1573,23 @@
       </c>
       <c r="B23" s="2">
         <f>B2</f>
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="C23" s="2">
         <f t="shared" ref="C23:F23" si="5">C2</f>
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="D23" s="2">
         <f t="shared" si="5"/>
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="E23" s="2">
         <f t="shared" si="5"/>
-        <v>13</v>
+        <v>20</v>
       </c>
       <c r="F23" s="2">
         <f t="shared" si="5"/>
-        <v>14</v>
+        <v>24</v>
       </c>
     </row>
     <row r="24" spans="1:15" ht="18.75" x14ac:dyDescent="0.3">
@@ -1520,21 +1597,11 @@
         <f>A17</f>
         <v>20</v>
       </c>
-      <c r="B24" s="3">
-        <v>7</v>
-      </c>
-      <c r="C24" s="3">
-        <v>5</v>
-      </c>
-      <c r="D24" s="3">
-        <v>8</v>
-      </c>
-      <c r="E24" s="3">
-        <v>9</v>
-      </c>
-      <c r="F24" s="3">
-        <v>12</v>
-      </c>
+      <c r="B24" s="3"/>
+      <c r="C24" s="3"/>
+      <c r="D24" s="3"/>
+      <c r="E24" s="3"/>
+      <c r="F24" s="3"/>
     </row>
     <row r="25" spans="1:15" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A25" s="2">
@@ -1574,23 +1641,23 @@
       </c>
       <c r="B30" s="2">
         <f>B9</f>
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="C30" s="2">
         <f t="shared" ref="C30:F30" si="7">C9</f>
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="D30" s="2">
         <f t="shared" si="7"/>
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="E30" s="2">
         <f t="shared" si="7"/>
-        <v>13</v>
+        <v>20</v>
       </c>
       <c r="F30" s="2">
         <f t="shared" si="7"/>
-        <v>14</v>
+        <v>24</v>
       </c>
       <c r="O30">
         <f>2/0.17</f>
@@ -1602,21 +1669,11 @@
         <f>A24</f>
         <v>20</v>
       </c>
-      <c r="B31" s="3">
-        <v>1</v>
-      </c>
-      <c r="C31" s="3">
-        <v>2</v>
-      </c>
-      <c r="D31" s="3">
-        <v>2</v>
-      </c>
-      <c r="E31" s="3">
-        <v>2</v>
-      </c>
-      <c r="F31" s="3">
-        <v>2</v>
-      </c>
+      <c r="B31" s="3"/>
+      <c r="C31" s="3"/>
+      <c r="D31" s="3"/>
+      <c r="E31" s="3"/>
+      <c r="F31" s="3"/>
     </row>
     <row r="32" spans="1:15" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A32" s="2">
@@ -1657,10 +1714,28 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="L20" sqref="L20"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H14" sqref="H14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
2 mins for 10-parties PSI
</commit_message>
<xml_diff>
--- a/stash size.xlsx
+++ b/stash size.xlsx
@@ -9,13 +9,18 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12210" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12210" activeTab="8"/>
   </bookViews>
   <sheets>
     <sheet name="2 hashes" sheetId="2" r:id="rId1"/>
     <sheet name="3 hashes" sheetId="1" r:id="rId2"/>
-    <sheet name="16" sheetId="3" r:id="rId3"/>
-    <sheet name="12" sheetId="4" r:id="rId4"/>
+    <sheet name="20" sheetId="5" r:id="rId3"/>
+    <sheet name="16" sheetId="3" r:id="rId4"/>
+    <sheet name="12" sheetId="4" r:id="rId5"/>
+    <sheet name="4 parties" sheetId="6" r:id="rId6"/>
+    <sheet name="5p" sheetId="7" r:id="rId7"/>
+    <sheet name="8p" sheetId="8" r:id="rId8"/>
+    <sheet name="10" sheetId="9" r:id="rId9"/>
   </sheets>
   <calcPr calcId="171027"/>
   <extLst>
@@ -27,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="13">
   <si>
     <t>n/trial</t>
   </si>
@@ -63,6 +68,9 @@
   </si>
   <si>
     <t>1.15n bins</t>
+  </si>
+  <si>
+    <t>trieun@onid.oregonstate.edu</t>
   </si>
 </sst>
 </file>
@@ -209,6 +217,55 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>18362</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>66595</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Picture 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{CAD772AA-CA97-422D-8D53-C3F7FA5E86EE}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="5504762" cy="638095"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
       <xdr:colOff>257175</xdr:colOff>
       <xdr:row>0</xdr:row>
       <xdr:rowOff>114300</xdr:rowOff>
@@ -253,7 +310,7 @@
 </xdr:wsDr>
 </file>
 
-<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
@@ -291,6 +348,202 @@
         <a:xfrm>
           <a:off x="0" y="0"/>
           <a:ext cx="3447619" cy="1580952"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing4.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>132876</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>152095</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Picture 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{70B44C0B-F0D5-44D6-97E9-BDE81780FEE2}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="3790476" cy="2438095"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing5.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>409575</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>361423</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>94881</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Picture 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B836F3B9-DF41-496E-A518-D5BFCC5422F8}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="409575" y="0"/>
+          <a:ext cx="4219048" cy="2952381"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing6.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>409143</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>142500</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Picture 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{ACBB8CF0-53C7-4132-B55C-D009186E52BA}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="3457143" cy="3000000"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing7.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>275733</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>9071</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Picture 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8B6AC9A2-9A29-44FF-AA31-826BF8B2B732}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="0" y="190500"/>
+          <a:ext cx="3933333" cy="3628571"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1714,9 +1967,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="L20" sqref="L20"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
@@ -1729,7 +1980,22 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
+      <selection activeCell="L20" sqref="L20"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
       <selection activeCell="H14" sqref="H14"/>
     </sheetView>
   </sheetViews>
@@ -1738,4 +2004,70 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F22" sqref="F22"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="K15" sqref="K15"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="H26"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H26" sqref="H26"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="26" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H26" t="s">
+        <v>12</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I19" sqref="I19"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>